<commit_message>
create and write in PDf file
</commit_message>
<xml_diff>
--- a/users.xlsx
+++ b/users.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -28,34 +28,10 @@
     <t xml:space="preserve">dob</t>
   </si>
   <si>
-    <t xml:space="preserve">Pravin</t>
+    <t xml:space="preserve">Hari</t>
   </si>
   <si>
-    <t xml:space="preserve">14-02-1998</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dilli</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27-03-1996</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sanjay</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15-06-1997</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yohesh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10-08-1997</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pravin Kumar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">03-08-1997</t>
+    <t xml:space="preserve">31-10-1999</t>
   </si>
 </sst>
 </file>
@@ -70,6 +46,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -151,10 +128,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -178,38 +155,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>